<commit_message>
Added a check for multiple bot replies to same comment
Before a bot replies to a comment, check the comment for any replies
from bot.
</commit_message>
<xml_diff>
--- a/opinions.xlsx
+++ b/opinions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmauermannpeterson/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmauermannpeterson/GitHub/reddit-bot-opinionated/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Donald Trump</t>
   </si>
@@ -62,18 +62,12 @@
     <t>Nintendo</t>
   </si>
   <si>
-    <t>Poop</t>
-  </si>
-  <si>
     <t>Grumpy Cat</t>
   </si>
   <si>
     <t>Doge</t>
   </si>
   <si>
-    <t>Spongebob</t>
-  </si>
-  <si>
     <t>Mexico</t>
   </si>
   <si>
@@ -125,9 +119,6 @@
     <t>Washington</t>
   </si>
   <si>
-    <t>Football</t>
-  </si>
-  <si>
     <t>life itself</t>
   </si>
   <si>
@@ -144,6 +135,42 @@
   </si>
   <si>
     <t>napping</t>
+  </si>
+  <si>
+    <t>RuPaul</t>
+  </si>
+  <si>
+    <t>Valentina</t>
+  </si>
+  <si>
+    <t>Willam</t>
+  </si>
+  <si>
+    <t>Sharon Needles</t>
+  </si>
+  <si>
+    <t>Alyssa Edwards</t>
+  </si>
+  <si>
+    <t>Whataburger</t>
+  </si>
+  <si>
+    <t>In-N-Out</t>
+  </si>
+  <si>
+    <t>football</t>
+  </si>
+  <si>
+    <t>SpongeBob</t>
+  </si>
+  <si>
+    <t>poop</t>
+  </si>
+  <si>
+    <t>Star Wars</t>
+  </si>
+  <si>
+    <t>Star Trek</t>
   </si>
 </sst>
 </file>
@@ -459,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A39"/>
+  <dimension ref="A1:A48"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,142 +551,187 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more opinion terms
</commit_message>
<xml_diff>
--- a/opinions.xlsx
+++ b/opinions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Donald Trump</t>
   </si>
@@ -171,6 +171,81 @@
   </si>
   <si>
     <t>Star Trek</t>
+  </si>
+  <si>
+    <t>a liberal</t>
+  </si>
+  <si>
+    <t>a conservative</t>
+  </si>
+  <si>
+    <t>my mom</t>
+  </si>
+  <si>
+    <t>your mom</t>
+  </si>
+  <si>
+    <t>covfefe</t>
+  </si>
+  <si>
+    <t>a can of cold spaghettiOs</t>
+  </si>
+  <si>
+    <t>cracking open a cold one with the boys</t>
+  </si>
+  <si>
+    <t>Super Mario 64</t>
+  </si>
+  <si>
+    <t>Breath of the Wild</t>
+  </si>
+  <si>
+    <t>Princess Peach</t>
+  </si>
+  <si>
+    <t>Luigi</t>
+  </si>
+  <si>
+    <t>Final Fantasy VIII</t>
+  </si>
+  <si>
+    <t>Final Fantasy VII</t>
+  </si>
+  <si>
+    <t>Final Fantasy IX</t>
+  </si>
+  <si>
+    <t>Donkey Kong</t>
+  </si>
+  <si>
+    <t>Ocarina of Time</t>
+  </si>
+  <si>
+    <t>A Link to the Past</t>
+  </si>
+  <si>
+    <t>Gamecube</t>
+  </si>
+  <si>
+    <t>Pokemon</t>
+  </si>
+  <si>
+    <t>that picture you posted on /gonewild</t>
+  </si>
+  <si>
+    <t>your face</t>
+  </si>
+  <si>
+    <t>the Jolly Rancher story</t>
+  </si>
+  <si>
+    <t>the Doritos story</t>
+  </si>
+  <si>
+    <t>that story about the broken arms</t>
+  </si>
+  <si>
+    <t>the gay agenda</t>
   </si>
 </sst>
 </file>
@@ -486,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A48"/>
+  <dimension ref="A1:A73"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -734,6 +809,131 @@
         <v>47</v>
       </c>
     </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed grammar of various opinion terms
</commit_message>
<xml_diff>
--- a/opinions.xlsx
+++ b/opinions.xlsx
@@ -50,9 +50,6 @@
     <t>Android</t>
   </si>
   <si>
-    <t>iPhone</t>
-  </si>
-  <si>
     <t>Micro$oft</t>
   </si>
   <si>
@@ -242,9 +239,6 @@
     <t>the Doritos story</t>
   </si>
   <si>
-    <t>that story about the broken arms</t>
-  </si>
-  <si>
     <t>the gay agenda</t>
   </si>
   <si>
@@ -309,6 +303,12 @@
   </si>
   <si>
     <t>an attack Widowmaker</t>
+  </si>
+  <si>
+    <t>the iPhone</t>
+  </si>
+  <si>
+    <t>that story about the kid with broken arms and his mom</t>
   </si>
 </sst>
 </file>
@@ -646,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A94"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,437 +689,437 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>